<commit_message>
Enhance Chart of Accounts import/export functionality with improved testing and error handling.  Includes updated test files, scripts, and documentation.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 37073a04-5ad1-4aa0-924c-d999899fb88e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/80550fad-9a85-4035-aa54-a26530837091/dcdf275a-c10d-407e-a7e6-8723c59c74d9.jpg
</commit_message>
<xml_diff>
--- a/test/coa-import-export/invalid_import.xlsx
+++ b/test/coa-import-export/invalid_import.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,68 +436,86 @@
         <v>1000</v>
       </c>
       <c r="B2" t="str">
-        <v>Cash</v>
+        <v>Invalid Type</v>
       </c>
       <c r="C2" t="str">
-        <v>ASSET</v>
+        <v>INVALID_TYPE</v>
       </c>
       <c r="D2" t="str">
         <v>Current Asset</v>
       </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
+      <c r="E2" t="str">
+        <v>false</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v>true</v>
       </c>
       <c r="H2" t="str">
-        <v>Cash on hand</v>
+        <v>Invalid account type</v>
+      </c>
+      <c r="I2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="B3" t="str">
-        <v>Cash Duplicate</v>
+        <v/>
       </c>
       <c r="C3" t="str">
-        <v>ASSET</v>
+        <v>LIABILITY</v>
       </c>
       <c r="D3" t="str">
-        <v>Current Asset</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
+        <v>Current Liability</v>
+      </c>
+      <c r="E3" t="str">
+        <v>false</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v>true</v>
       </c>
       <c r="H3" t="str">
-        <v>Duplicate cash account</v>
+        <v>Missing name field</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2000</v>
+        <v>3000</v>
+      </c>
+      <c r="B4" t="str">
+        <v>First Equity Account</v>
       </c>
       <c r="C4" t="str">
-        <v>LIABILITY</v>
+        <v>EQUITY</v>
       </c>
       <c r="D4" t="str">
-        <v>Current Liability</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
+        <v>Equity</v>
+      </c>
+      <c r="E4" t="str">
+        <v>false</v>
       </c>
       <c r="F4" t="str">
-        <v>Vendor</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v>true</v>
       </c>
       <c r="H4" t="str">
-        <v>Accounts payable</v>
+        <v>First equity account with code 3000</v>
+      </c>
+      <c r="I4" t="str">
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -505,30 +523,36 @@
         <v>3000</v>
       </c>
       <c r="B5" t="str">
-        <v>Equity</v>
+        <v>Duplicate Code</v>
       </c>
       <c r="C5" t="str">
-        <v>INVALID_TYPE</v>
+        <v>EQUITY</v>
       </c>
       <c r="D5" t="str">
         <v>Equity</v>
       </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
+      <c r="E5" t="str">
+        <v>false</v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v>true</v>
       </c>
       <c r="H5" t="str">
-        <v>Equity account</v>
+        <v>Duplicate code 3000</v>
+      </c>
+      <c r="I5" t="str">
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>4100</v>
+        <v>4000</v>
       </c>
       <c r="B6" t="str">
-        <v>Product Sales</v>
+        <v>Invalid Parent</v>
       </c>
       <c r="C6" t="str">
         <v>REVENUE</v>
@@ -536,14 +560,17 @@
       <c r="D6" t="str">
         <v>Operating Revenue</v>
       </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
+      <c r="E6" t="str">
+        <v>false</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v>true</v>
       </c>
       <c r="H6" t="str">
-        <v>Revenue from product sales</v>
+        <v>Invalid parent code</v>
       </c>
       <c r="I6" t="str">
         <v>9999</v>
@@ -551,33 +578,65 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>5000</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Parent Account</v>
+      </c>
+      <c r="C7" t="str">
+        <v>EXPENSE</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Operating Expense</v>
+      </c>
+      <c r="E7" t="str">
+        <v>false</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v>true</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Parent account</v>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
         <v>5100</v>
       </c>
-      <c r="B7" t="str">
-        <v>Child COGS</v>
-      </c>
-      <c r="C7" t="str">
-        <v>ASSET</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Cost of Sales</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Child COGS account</v>
-      </c>
-      <c r="I7" t="str">
+      <c r="B8" t="str">
+        <v>Type Mismatch</v>
+      </c>
+      <c r="C8" t="str">
+        <v>REVENUE</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Operating Revenue</v>
+      </c>
+      <c r="E8" t="str">
+        <v>false</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>true</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Type mismatch with parent</v>
+      </c>
+      <c r="I8" t="str">
         <v>5000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>